<commit_message>
fix: new zero daily
</commit_message>
<xml_diff>
--- a/daily released.xlsx
+++ b/daily released.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liang/code/shanghai-2022Mar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE947BAD-035A-1649-A45F-D0B8EE928E28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67269B1-98BF-C041-8746-11DD24194A01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="1480" windowWidth="19840" windowHeight="13820" xr2:uid="{B61748C7-A350-CD4C-8140-E3EEE49B7E25}"/>
   </bookViews>
   <sheets>
-    <sheet name="0422" sheetId="1" r:id="rId1"/>
+    <sheet name="0423" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -498,7 +498,7 @@
   <dimension ref="A1:AG20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -607,6 +607,9 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="J2">
+        <v>230</v>
+      </c>
       <c r="K2">
         <v>134</v>
       </c>
@@ -678,6 +681,9 @@
     <row r="3" spans="1:33">
       <c r="A3" t="s">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>29</v>
       </c>
       <c r="K3">
         <v>140</v>
@@ -751,6 +757,9 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="J4">
+        <v>51</v>
+      </c>
       <c r="K4">
         <v>43</v>
       </c>
@@ -822,6 +831,9 @@
     <row r="5" spans="1:33">
       <c r="A5" t="s">
         <v>3</v>
+      </c>
+      <c r="J5">
+        <v>35</v>
       </c>
       <c r="K5">
         <v>64</v>
@@ -895,6 +907,9 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="J6">
+        <v>48</v>
+      </c>
       <c r="K6">
         <v>50</v>
       </c>
@@ -967,6 +982,9 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="J7">
+        <v>35</v>
+      </c>
       <c r="K7">
         <v>37</v>
       </c>
@@ -1039,6 +1057,9 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
       <c r="K8">
         <v>44</v>
       </c>
@@ -1111,6 +1132,9 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="J9">
+        <v>74</v>
+      </c>
       <c r="K9">
         <v>44</v>
       </c>
@@ -1183,6 +1207,9 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="J10">
+        <v>213</v>
+      </c>
       <c r="K10">
         <v>269</v>
       </c>
@@ -1255,6 +1282,9 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="J11">
+        <v>29</v>
+      </c>
       <c r="K11">
         <v>11</v>
       </c>
@@ -1327,6 +1357,9 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="J12">
+        <v>24</v>
+      </c>
       <c r="K12">
         <v>111</v>
       </c>
@@ -1399,6 +1432,9 @@
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="J13">
+        <v>8</v>
+      </c>
       <c r="K13">
         <v>9</v>
       </c>
@@ -1471,6 +1507,9 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="J14">
+        <v>47</v>
+      </c>
       <c r="K14">
         <v>65</v>
       </c>
@@ -1543,6 +1582,9 @@
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="J15">
+        <v>53</v>
+      </c>
       <c r="K15">
         <v>31</v>
       </c>
@@ -1615,6 +1657,9 @@
       <c r="A16" t="s">
         <v>14</v>
       </c>
+      <c r="J16">
+        <v>14</v>
+      </c>
       <c r="K16">
         <v>17</v>
       </c>
@@ -1687,6 +1732,9 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
       <c r="K17">
         <v>6</v>
       </c>
@@ -1759,6 +1807,9 @@
       <c r="A18" t="s">
         <v>16</v>
       </c>
+      <c r="J18">
+        <v>19621</v>
+      </c>
       <c r="K18">
         <v>18471</v>
       </c>
@@ -1833,6 +1884,9 @@
       <c r="A19" t="s">
         <v>17</v>
       </c>
+      <c r="J19">
+        <v>23336</v>
+      </c>
       <c r="K19">
         <v>23381</v>
       </c>
@@ -1906,6 +1960,9 @@
     <row r="20" spans="1:33">
       <c r="A20" t="s">
         <v>18</v>
+      </c>
+      <c r="J20">
+        <v>7814</v>
       </c>
       <c r="K20">
         <v>7029</v>

</xml_diff>